<commit_message>
removed ReportCard reference from StudentAcademicRecord, created AlternativeCourseIdentificationCode common in extension project and replaced original reference in CourseTranscript
</commit_message>
<xml_diff>
--- a/EdFiXTranscript/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
+++ b/EdFiXTranscript/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ed-Fi Handbook"/>
-  <dimension ref="A1:G697"/>
+  <dimension ref="A1:G698"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3399,7 +3399,6 @@
 IdentificationCode (required)
 Used By:
 Course.CourseIdentificationCode (as required collection)
-CourseTranscript.CourseIdentificationCode (as optional collection)
 CourseTranscript.CourseIdentificationCode (as optional collection)</v>
       </c>
     </row>
@@ -9087,6 +9086,7 @@
       <c r="G336" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
 CourseIdentificationCode.CourseIdentificationSystem (as identity)
+AlternativeCourseIdentificationCode.CourseIdentificationSystem (as identity)
 CourseTranscript.CourseIdentificationSystem (as identity)</v>
       </c>
     </row>
@@ -13777,7 +13777,6 @@
 StudentCompetencyObjective (optional collection)
 StudentLearningObjective (optional collection)
 Used By:
-StudentAcademicRecord.ReportCard (as optional collection)
 StudentAcademicRecord.ReportCard (as optional collection)</v>
       </c>
     </row>
@@ -18565,13 +18564,13 @@
         <v/>
       </c>
       <c r="B695" t="str">
-        <v>ProjectedGraduationDate</v>
+        <v>AlternativeCourseIdentificationCode (EdFiXTranscript)</v>
       </c>
       <c r="C695" t="str">
-        <v>The month and year the student is projected to graduate.</v>
+        <v>A standard code that identifies the organization of subject matter and related learning experiences provided for the instruction of students.</v>
       </c>
       <c r="D695" t="str">
-        <v>Date</v>
+        <v>Composite Part</v>
       </c>
       <c r="E695" t="str">
         <v/>
@@ -18580,8 +18579,13 @@
         <v/>
       </c>
       <c r="G695" t="str" xml:space="preserve">
-        <v xml:space="preserve">Used By:
-StudentAcademicRecord.ProjectedGraduationDate (as optional)</v>
+        <v xml:space="preserve">Contains:
+CourseCatalogURL (optional)
+CourseIdentificationSystem (identity)
+IdentificationCode (optional)
+IdentificationCode (required)
+Used By:
+CourseTranscript.AlternativeCourseIdentificationCode (as optional collection)</v>
       </c>
     </row>
     <row r="696" xml:space="preserve">
@@ -18589,29 +18593,53 @@
         <v/>
       </c>
       <c r="B696" t="str">
+        <v>ProjectedGraduationDate</v>
+      </c>
+      <c r="C696" t="str">
+        <v>The month and year the student is projected to graduate.</v>
+      </c>
+      <c r="D696" t="str">
+        <v>Date</v>
+      </c>
+      <c r="E696" t="str">
+        <v/>
+      </c>
+      <c r="F696" t="str">
+        <v/>
+      </c>
+      <c r="G696" t="str" xml:space="preserve">
+        <v xml:space="preserve">Used By:
+StudentAcademicRecord.ProjectedGraduationDate (as optional)</v>
+      </c>
+    </row>
+    <row r="697" xml:space="preserve">
+      <c r="A697" t="str">
+        <v/>
+      </c>
+      <c r="B697" t="str">
         <v>CourseTranscript (EdFiXTranscript)</v>
       </c>
-      <c r="C696" t="str">
+      <c r="C697" t="str">
         <v>This entity is the final record of a student's performance in their courses at the end of a semester or school year.</v>
       </c>
-      <c r="D696" t="str">
+      <c r="D697" t="str">
         <v>Class</v>
       </c>
-      <c r="E696" t="str">
-        <v/>
-      </c>
-      <c r="F696" t="str">
-        <v/>
-      </c>
-      <c r="G696" t="str" xml:space="preserve">
+      <c r="E697" t="str">
+        <v/>
+      </c>
+      <c r="F697" t="str">
+        <v/>
+      </c>
+      <c r="G697" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
 AcademicSubject (optional collection)
 AdditionalCredits (optional collection)
+AlternativeCourseIdentificationCode (optional collection)
 AlternativeCourseTitle (optional)
 Course (optional collection)
 CourseAttemptResult (identity)
 CourseCatalogURL (optional)
-CourseIdentificationCode (optional collection)
 CourseIdentificationSystem (identity)
 CourseRepeatCode (optional)
 CourseTitle (optional)
@@ -18628,26 +18656,26 @@
 StudentAcademicRecord (identity)</v>
       </c>
     </row>
-    <row r="697" xml:space="preserve">
-      <c r="A697" t="str">
-        <v/>
-      </c>
-      <c r="B697" t="str">
+    <row r="698" xml:space="preserve">
+      <c r="A698" t="str">
+        <v/>
+      </c>
+      <c r="B698" t="str">
         <v>StudentAcademicRecord (EdFiXTranscript)</v>
       </c>
-      <c r="C697" t="str">
+      <c r="C698" t="str">
         <v>This educational entity represents the cumulative record of academic achievement for a student.</v>
       </c>
-      <c r="D697" t="str">
+      <c r="D698" t="str">
         <v>Class</v>
       </c>
-      <c r="E697" t="str">
-        <v/>
-      </c>
-      <c r="F697" t="str">
-        <v/>
-      </c>
-      <c r="G697" t="str" xml:space="preserve">
+      <c r="E698" t="str">
+        <v/>
+      </c>
+      <c r="F698" t="str">
+        <v/>
+      </c>
+      <c r="G698" t="str" xml:space="preserve">
         <v xml:space="preserve">Contains:
 AcademicHonor (optional collection)
 ClassRanking (optional)
@@ -18660,7 +18688,6 @@
 GradePointAverage (optional collection)
 ProjectedGraduationDate (optional)
 Recognition (optional collection)
-ReportCard (optional collection)
 SchoolYear (identity)
 Student (identity)
 Term (identity)

</xml_diff>